<commit_message>
changed motor parameter stuff and PIDcontroller code
</commit_message>
<xml_diff>
--- a/ExperimentalData/MotorParameterData.xlsx
+++ b/ExperimentalData/MotorParameterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmvsu\OneDrive\Documents\School Winter 2018\elec 391\Laser-Light-Show\ExperimentalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E64201C-E9A5-43A6-9517-2035739AD1F4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1D5A8D-BA62-4F58-91CB-5FCA634355A8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="912" windowWidth="19200" windowHeight="7188" activeTab="1" xr2:uid="{453B5560-B02B-49E5-A604-6A12C721B6F9}"/>
+    <workbookView xWindow="0" yWindow="1368" windowWidth="19200" windowHeight="7188" activeTab="1" xr2:uid="{453B5560-B02B-49E5-A604-6A12C721B6F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -5213,7 +5213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C796C4-C56C-41DE-8C1B-9F60B7546137}">
   <dimension ref="A1:Q154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
       <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
@@ -5347,7 +5347,7 @@
         <v>-132</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E6:E69" si="0">(D10-D8)/(C10-C8)</f>
+        <f t="shared" ref="E9:E21" si="0">(D10-D8)/(C10-C8)</f>
         <v>-5.7</v>
       </c>
     </row>

</xml_diff>